<commit_message>
fixing fastqfilename in 480
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_480.xlsx
+++ b/fastqFiles/fastq_480.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">s_2_withindex_sequence_cir1_1_37CO2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_2_withindex_sequence_cir1_2_30.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">s_2_withindex_sequence_cir1_2_37CO2.fastq.gz</t>
@@ -89,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -119,6 +122,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,13 +179,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,8 +211,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,7 +442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>6</v>
       </c>
@@ -445,8 +458,8 @@
       <c r="E12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>10</v>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>